<commit_message>
Added graph of y = 3 cos x + 4 sin x
</commit_message>
<xml_diff>
--- a/MathLaTeX/MathNotes/TrigonometricFunctions.xlsx
+++ b/MathLaTeX/MathNotes/TrigonometricFunctions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonProjects\MLDataSci\MathLaTeX\MathNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E02A3C1-8688-42C3-A926-3C306472CA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6967629-6453-421E-8583-AD6366B7A414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15195" yWindow="4515" windowWidth="13620" windowHeight="11490" firstSheet="1" activeTab="4" xr2:uid="{F7E2AB23-6C4B-44A7-A5CC-1583FE09BB64}"/>
+    <workbookView xWindow="14175" yWindow="1380" windowWidth="13620" windowHeight="11490" firstSheet="2" activeTab="5" xr2:uid="{F7E2AB23-6C4B-44A7-A5CC-1583FE09BB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Frame 2" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Frame 7" sheetId="5" r:id="rId3"/>
     <sheet name="Frame 11" sheetId="6" r:id="rId4"/>
     <sheet name="Frame 25" sheetId="7" r:id="rId5"/>
+    <sheet name="Frame 28" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2062,6 +2063,449 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8EED-4B4B-A23D-86536D1A2C4B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="329541872"/>
+        <c:axId val="329546032"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="329541872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="329546032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="329546032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="329541872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-MY" i="1">
+                <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t>y</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-MY" baseline="0">
+                <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t> = 3 cos </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-MY" i="1" baseline="0">
+                <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t>x</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-MY" baseline="0">
+                <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t> + 4 sin </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-MY" i="1" baseline="0">
+                <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t>x</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-MY" baseline="30000">
+              <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:tint val="88500"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Frame 28'!$A$1:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Frame 28'!$B$1:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-0.34113014367187811</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.3818647266210569</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.3939330879193674</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.36623963184524255</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9981728527468015</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6866836550422324</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0662791186408769</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3.5344575220408054</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-4.8856302169441541</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.7449770216271667</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.9867908568360058</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3887491976612996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2.4054974575618675</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-4.9881408438225492</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2.9847105422628752</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7628488671553946</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.8896531579050695</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.5209328850676864</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.0849168446870043</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-4.6932990307868359</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9F70-4D8F-99A4-EDF7D1BE0D1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2359,6 +2803,33 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4424,6 +4895,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5154,6 +6141,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>305866</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>50133</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FD54FFB-538E-427A-A34E-74D71C847BC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6274,7 +7304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2E102E-1912-48F0-84C3-33DB17620E17}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -6473,4 +7503,212 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC21C752-E689-492E-8C8D-496C6B9CF4AC}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>-10</v>
+      </c>
+      <c r="B1">
+        <f>(3 * COS(A1)) + (4 * SIN(A1))</f>
+        <v>-0.34113014367187811</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-9</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B21" si="0">(3 * COS(A2)) + (4 * SIN(A2))</f>
+        <v>-4.3818647266210569</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-8</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>-4.3939330879193674</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-7</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>-0.36623963184524255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-6</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>3.9981728527468015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>4.6866836550422324</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-4</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>1.0662791186408769</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-3</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>-3.5344575220408054</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-2</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>-4.8856302169441541</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-1</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>-1.7449770216271667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>4.9867908568360058</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>2.3887491976612996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>-2.4054974575618675</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>-4.9881408438225492</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>-2.9847105422628752</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>1.7628488671553946</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>4.8896531579050695</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>3.5209328850676864</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>-1.0849168446870043</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>-4.6932990307868359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>